<commit_message>
Co-pilot is pretty dope....
</commit_message>
<xml_diff>
--- a/Macro_Chartist/TemplateList.xlsx
+++ b/Macro_Chartist/TemplateList.xlsx
@@ -443,91 +443,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Financial conditions &amp; employment, US.xlsx</t>
+          <t>Bitcoin price change is fueled by global monetary growth (with forecast).xlsx</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bitty, SPX &amp; GM2 fitted trends.xlsx</t>
+          <t>Bank credit and M2 U.S.xlsx</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Monetary Expansion and Risk Asset Activity.xlsx</t>
+          <t>U.S GDP and GDI.xlsx</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Personal savings U.S (BEA).xlsx</t>
+          <t>US financial conditions, employment &amp; equities.xlsx</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bitcoin price change is fueled by global monetary growth.xlsx</t>
+          <t>Real Incomes U.S (BEA).xlsx</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>U.S GDP and GDI.xlsx</t>
+          <t>Bitty, SPX &amp; GM2 fitted trends.xlsx</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Real Incomes U.S (BEA).xlsx</t>
+          <t>Monetary Expansion and Risk Asset Activity.xlsx</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bitcoin price change is fueled by global monetary growth (with forecast).xlsx</t>
+          <t>US Equity Indices.xlsx</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>US financial conditions, employment &amp; equities.xlsx</t>
+          <t>US and Global Monetary Aggregates.xlsx</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>US Equity Indices.xlsx</t>
+          <t>Financial conditions &amp; employment, US.xlsx</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>US Gross Domestic Income and Equity Indices.xlsx</t>
+          <t>Bitcoin price change is fueled by global monetary growth.xlsx</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>US and Global Monetary Aggregates.xlsx</t>
+          <t>Personal savings U.S (BEA).xlsx</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Bank credit and M2 U.S.xlsx</t>
+          <t>Monetary Aggregates &amp; Inflation, USA.xlsx</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Monetary Aggregates &amp; Inflation, USA.xlsx</t>
+          <t>US Gross Domestic Income and Equity Indices.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>